<commit_message>
Update consul for service discovery(service registration/deregistration) and api gatewaya config update
</commit_message>
<xml_diff>
--- a/docs/Project Management.xlsx
+++ b/docs/Project Management.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
-    <sheet name="Backend - API Gateway" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Architecture" sheetId="4" r:id="rId2"/>
+    <sheet name="Backend - API Gateway" sheetId="1" r:id="rId3"/>
+    <sheet name="Backend - Auth" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>REALWorks Project Management - Summary</t>
   </si>
@@ -49,13 +50,58 @@
   </si>
   <si>
     <t>Setup complete configuration.json for Routes</t>
+  </si>
+  <si>
+    <t>Setup Service Discovery with Consul</t>
+  </si>
+  <si>
+    <t>Download and install consul, enable Ocelot to use consul, register services successfully with proof of concept with Backend - Asset Management Service</t>
+  </si>
+  <si>
+    <t>Split Ocelot configuration files as multiple files and merge when Ocelot starts.</t>
+  </si>
+  <si>
+    <t>Ocelot aggreagation</t>
+  </si>
+  <si>
+    <t>Updated On</t>
+  </si>
+  <si>
+    <t>Tested successfully integrating with consul using Asset Management Services (proof of concelp, to be implemented on other services)</t>
+  </si>
+  <si>
+    <t>Dynamic routing</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Proof of concept, more needs to be done for integrated testing</t>
+  </si>
+  <si>
+    <t>Health Check</t>
+  </si>
+  <si>
+    <t>On API Gateway, it needs to make sure service discovery with consul working well as well as general system health check.</t>
+  </si>
+  <si>
+    <t>REALWorks Project Management - Architecure Design</t>
+  </si>
+  <si>
+    <t>Ocelot configuration for Asset Services and Marketing Services</t>
+  </si>
+  <si>
+    <t>Configuration is completed, to be fully tested (GET test ok)</t>
+  </si>
+  <si>
+    <t>Will test POST operations with testing tool (Postman/VSCode RestClient) after review of both services implementation.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +139,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +171,11 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -128,13 +186,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -169,11 +228,39 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,6 +562,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -483,7 +588,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -491,12 +596,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,15 +609,16 @@
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -526,10 +632,13 @@
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -542,9 +651,10 @@
       <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="6"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -553,360 +663,466 @@
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="9"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="16">
+        <v>43656</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>3.1</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="18">
+        <v>43656</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>3.2</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>3.3</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
+        <v>3.4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="16">
+        <v>43661</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>4</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="3"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="3"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="3"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="3"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="3"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="3"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="3"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="3"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="3"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="3"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="3"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="3"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="3"/>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="3"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="3"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="3"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="3"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="3"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="3"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="3"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="3"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="3"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="3"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="3"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="3"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="5"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="3"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="5"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="3"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="5"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="3"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="3"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="5"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="3"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="5"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="5"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="3"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="5"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="3"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="5"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="3"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="5"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="3"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="5"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="3"/>
+      <c r="F55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="5"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -914,7 +1130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>